<commit_message>
Add import costs from cbip
</commit_message>
<xml_diff>
--- a/resources/Diggers Factory - Orders Shipping Costs.xlsx
+++ b/resources/Diggers Factory - Orders Shipping Costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vico/Sites/diggers/api/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38BA276-86EE-4043-A2E2-A720947B12FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC07C9C-B816-4C4A-B219-E64895CD86EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7880" yWindow="3860" windowWidth="29920" windowHeight="18660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -33,20 +33,14 @@
     <t>ID</t>
   </si>
   <si>
-    <t>INVOICE</t>
-  </si>
-  <si>
     <t>COST</t>
-  </si>
-  <si>
-    <t>I123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,10 +62,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF314750"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color rgb="FF545454"/>
+      <name val="Inter"/>
     </font>
   </fonts>
   <fills count="2">
@@ -105,12 +98,10 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,44 +406,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="21.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="23.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5">
+        <v>394732</v>
+      </c>
+      <c r="B2" s="2">
+        <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
-        <v>5477</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>